<commit_message>
added stats day 7 lecture files + calculator
</commit_message>
<xml_diff>
--- a/Statistics/Valerio_ExcelCalculator.xlsx
+++ b/Statistics/Valerio_ExcelCalculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skyla\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marshmerry/Desktop/SkyVale_Repo/Statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B4F933B-DA5F-48CD-A23B-C5057DA76890}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85ED54D-EBDF-974C-ACF8-D3A5D690AD71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3AFDB78A-A2A3-4F6B-A971-0F514BB2AA5B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24100" windowHeight="19060" xr2:uid="{3AFDB78A-A2A3-4F6B-A971-0F514BB2AA5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
   <si>
     <t>Binomial Distribution</t>
   </si>
@@ -133,13 +133,82 @@
   </si>
   <si>
     <t>Minimum Sample Size for Proportion Sampling</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>confidence</t>
+  </si>
+  <si>
+    <t>degrees of freedom</t>
+  </si>
+  <si>
+    <t>success percentage</t>
+  </si>
+  <si>
+    <t>failure percentage</t>
+  </si>
+  <si>
+    <t>margin of error</t>
+  </si>
+  <si>
+    <t>KEY</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">t-value </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(intersection of c + df on the t-chart)</t>
+    </r>
+  </si>
+  <si>
+    <t>z-score of confidence % (look at chart)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">standard deviation </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(NOT sample stdev)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,8 +244,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,8 +293,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -251,6 +345,68 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -268,7 +424,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -313,7 +469,50 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="5" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -635,52 +834,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF320F6-FD0A-4282-BA0B-51E223412FFB}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="13"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -689,7 +891,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -698,7 +900,10 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
+      <c r="A11" s="18"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -707,7 +912,7 @@
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="14" t="s">
         <v>9</v>
       </c>
@@ -724,7 +929,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
         <v>1</v>
       </c>
@@ -741,13 +946,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="E15" s="7" t="e">
         <f>D15/SQRT(A15)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
@@ -756,7 +961,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="12" t="s">
         <v>19</v>
       </c>
@@ -764,7 +969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="11">
         <v>0.9</v>
       </c>
@@ -772,7 +977,7 @@
         <v>1.645</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="11">
         <v>0.95</v>
       </c>
@@ -780,7 +985,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="11">
         <v>0.99</v>
       </c>
@@ -788,7 +993,12 @@
         <v>2.5750000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
+      <c r="A24" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
@@ -797,7 +1007,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="4" t="s">
         <v>1</v>
       </c>
@@ -811,13 +1021,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="9"/>
       <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H27" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="39"/>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="4" t="s">
         <v>24</v>
       </c>
@@ -827,8 +1044,17 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H28" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="34"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="28"/>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
@@ -838,8 +1064,17 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H29" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="J29" s="34"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="28"/>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
@@ -849,8 +1084,42 @@
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H30" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" s="34"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="28"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="H31" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="J31" s="34"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="28"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="J32" s="34"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="28"/>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="3" t="s">
         <v>25</v>
       </c>
@@ -858,8 +1127,17 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H33" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="I33" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="J33" s="34"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="28"/>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="4" t="s">
         <v>24</v>
       </c>
@@ -869,23 +1147,72 @@
       <c r="C34" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="9"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H34" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="I34" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="J34" s="34"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="28"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="B35" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="C35" s="9">
+        <v>1.645</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="I35" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="J35" s="34"/>
+      <c r="K35" s="27"/>
+      <c r="L35" s="28"/>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="4" t="e">
+      <c r="B36" s="26">
         <f>(C35*B35/A35)^2</f>
-        <v>#DIV/0!</v>
+        <v>2770.9695999999999</v>
       </c>
       <c r="C36" s="1"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H36" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="J36" s="34"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="28"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="H37" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="I37" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="J37" s="36"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="30"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" s="3" t="s">
         <v>26</v>
       </c>
@@ -895,15 +1222,15 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>27</v>
@@ -915,45 +1242,60 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="9"/>
+    <row r="41" spans="1:12">
+      <c r="A41" s="4">
+        <v>123</v>
+      </c>
+      <c r="B41" s="4">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.84</v>
+      </c>
+      <c r="D41" s="11">
+        <v>0.95</v>
+      </c>
+      <c r="E41" s="9">
+        <v>1.984</v>
+      </c>
       <c r="F41" s="4">
         <f>A41-1</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="4" t="e">
+      <c r="B42" s="20">
         <f>E41*C41/SQRT(A41)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.15026865463513558</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="4" t="e">
+      <c r="B43" s="20">
         <f>B41-B42</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8.0497313453648633</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="4" t="e">
+      <c r="B44" s="20">
         <f>B41+B42</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8.3502686546351352</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" s="3" t="s">
         <v>32</v>
       </c>
@@ -963,7 +1305,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="A48" s="4" t="s">
         <v>1</v>
       </c>
@@ -980,55 +1322,67 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4" t="e">
+    <row r="49" spans="1:5">
+      <c r="A49" s="4">
+        <v>1345</v>
+      </c>
+      <c r="B49" s="4">
+        <v>345</v>
+      </c>
+      <c r="C49" s="19">
         <f>B49/A49</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D49" s="4" t="e">
+        <v>0.25650557620817843</v>
+      </c>
+      <c r="D49" s="19">
         <f>1-C49</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E49" s="9"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.74349442379182151</v>
+      </c>
+      <c r="E49" s="9">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B50" s="4" t="e">
-        <f>E40*SQRT(C49*D49/A49)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="19">
+        <f>E49*SQRT(C49*D49/A49)</f>
+        <v>2.3338997225887365E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B51" s="4" t="e">
+      <c r="B51" s="19">
         <f>C49-B50</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.23316657898229107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="4" t="e">
+      <c r="B52" s="19">
         <f>C49+B50</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="18" t="s">
+        <v>0.27984457343406577</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D55" s="23"/>
+      <c r="E55" s="24"/>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="10" t="s">
         <v>3</v>
       </c>
@@ -1042,29 +1396,36 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
+    <row r="57" spans="1:5">
+      <c r="A57" s="4">
+        <v>0.5</v>
+      </c>
       <c r="B57" s="4">
         <f>1-A57</f>
-        <v>1</v>
-      </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="9"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="C57" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="D57" s="9">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B58" s="4" t="e">
+      <c r="B58" s="25">
         <f>A57*B57*(D57/C57)^2</f>
-        <v>#DIV/0!</v>
+        <v>384.15999999999991</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="H27:L27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added stats assignment 7
</commit_message>
<xml_diff>
--- a/Statistics/Valerio_ExcelCalculator.xlsx
+++ b/Statistics/Valerio_ExcelCalculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marshmerry/Desktop/SkyVale_Repo/Statistics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skyla\OneDrive\Desktop\SkyVale_Repo\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85ED54D-EBDF-974C-ACF8-D3A5D690AD71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7426A0D-5FD4-47A6-839D-50AAED871152}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24100" windowHeight="19060" xr2:uid="{3AFDB78A-A2A3-4F6B-A971-0F514BB2AA5B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3AFDB78A-A2A3-4F6B-A971-0F514BB2AA5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -205,8 +205,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -466,16 +466,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -506,6 +503,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -836,21 +836,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF320F6-FD0A-4282-BA0B-51E223412FFB}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="13" t="s">
@@ -901,7 +901,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="18"/>
+      <c r="A11" s="17"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
@@ -994,7 +994,7 @@
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="21" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1022,10 +1022,18 @@
       </c>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="4"/>
+      <c r="A27" s="4">
+        <v>35</v>
+      </c>
+      <c r="B27" s="4">
+        <v>30.87</v>
+      </c>
+      <c r="C27" s="9">
+        <v>1.645</v>
+      </c>
+      <c r="D27" s="4">
+        <v>150.27000000000001</v>
+      </c>
       <c r="H27" s="37" t="s">
         <v>45</v>
       </c>
@@ -1038,86 +1046,86 @@
       <c r="A28" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="4" t="e">
+      <c r="B28" s="4">
         <f>C27*B27/SQRT(A27)</f>
-        <v>#DIV/0!</v>
+        <v>8.5835809965014018</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="H28" s="31" t="s">
+      <c r="H28" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="I28" s="33" t="s">
+      <c r="I28" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="J28" s="34"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="28"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="27"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="4" t="e">
+      <c r="B29" s="4">
         <f>D27-B28</f>
-        <v>#DIV/0!</v>
+        <v>141.6864190034986</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="H29" s="31" t="s">
+      <c r="H29" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="I29" s="33" t="s">
+      <c r="I29" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="J29" s="34"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="28"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="27"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="4" t="e">
+      <c r="B30" s="4">
         <f>D27+B28</f>
-        <v>#DIV/0!</v>
+        <v>158.85358099650142</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="H30" s="31" t="s">
+      <c r="H30" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="33" t="s">
+      <c r="I30" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="J30" s="34"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="28"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="27"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="H31" s="31" t="s">
+      <c r="H31" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="I31" s="33" t="s">
+      <c r="I31" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="J31" s="34"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="28"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="27"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H32" s="31" t="s">
+      <c r="H32" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="I32" s="33" t="s">
+      <c r="I32" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="J32" s="34"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="28"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="27"/>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="3" t="s">
@@ -1127,15 +1135,15 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="H33" s="31" t="s">
+      <c r="H33" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="I33" s="33" t="s">
+      <c r="I33" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="J33" s="34"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="28"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="27"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="4" t="s">
@@ -1147,68 +1155,68 @@
       <c r="C34" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H34" s="31" t="s">
+      <c r="H34" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="I34" s="33" t="s">
+      <c r="I34" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="J34" s="34"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="28"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="27"/>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="B35" s="4">
-        <v>3.2</v>
+        <v>4.8</v>
       </c>
       <c r="C35" s="9">
-        <v>1.645</v>
-      </c>
-      <c r="H35" s="31" t="s">
+        <v>1.96</v>
+      </c>
+      <c r="H35" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I35" s="33" t="s">
+      <c r="I35" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="J35" s="34"/>
-      <c r="K35" s="27"/>
-      <c r="L35" s="28"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="26"/>
+      <c r="L35" s="27"/>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="26">
+      <c r="B36" s="25">
         <f>(C35*B35/A35)^2</f>
-        <v>2770.9695999999999</v>
+        <v>88.510463999999985</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="H36" s="31" t="s">
+      <c r="H36" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I36" s="33" t="s">
+      <c r="I36" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="J36" s="34"/>
-      <c r="K36" s="27"/>
-      <c r="L36" s="28"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="27"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="H37" s="32" t="s">
+      <c r="H37" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="I37" s="35" t="s">
+      <c r="I37" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="J37" s="36"/>
-      <c r="K37" s="29"/>
-      <c r="L37" s="30"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="29"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="20" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1244,54 +1252,54 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="4">
-        <v>123</v>
+        <v>14</v>
       </c>
       <c r="B41" s="4">
-        <v>8.1999999999999993</v>
+        <v>64</v>
       </c>
       <c r="C41" s="4">
-        <v>0.84</v>
+        <v>9</v>
       </c>
       <c r="D41" s="11">
-        <v>0.95</v>
+        <v>0.98</v>
       </c>
       <c r="E41" s="9">
-        <v>1.984</v>
+        <v>2.65</v>
       </c>
       <c r="F41" s="4">
         <f>A41-1</f>
-        <v>122</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B42" s="20">
+      <c r="B42" s="19">
         <f>E41*C41/SQRT(A41)</f>
-        <v>0.15026865463513558</v>
+        <v>6.3741806196113213</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="20">
+      <c r="B43" s="19">
         <f>B41-B42</f>
-        <v>8.0497313453648633</v>
+        <v>57.625819380388677</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="20">
+      <c r="B44" s="19">
         <f>B41+B42</f>
-        <v>8.3502686546351352</v>
+        <v>70.374180619611323</v>
       </c>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="21" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1324,52 +1332,52 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="4">
-        <v>1345</v>
+        <v>200</v>
       </c>
       <c r="B49" s="4">
-        <v>345</v>
-      </c>
-      <c r="C49" s="19">
+        <v>154</v>
+      </c>
+      <c r="C49" s="18">
         <f>B49/A49</f>
-        <v>0.25650557620817843</v>
-      </c>
-      <c r="D49" s="19">
+        <v>0.77</v>
+      </c>
+      <c r="D49" s="18">
         <f>1-C49</f>
-        <v>0.74349442379182151</v>
+        <v>0.22999999999999998</v>
       </c>
       <c r="E49" s="9">
-        <v>1.96</v>
+        <v>1.645</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B50" s="19">
+      <c r="B50" s="18">
         <f>E49*SQRT(C49*D49/A49)</f>
-        <v>2.3338997225887365E-2</v>
+        <v>4.8950844093845813E-2</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B51" s="19">
+      <c r="B51" s="18">
         <f>C49-B50</f>
-        <v>0.23316657898229107</v>
+        <v>0.72104915590615426</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B52" s="19">
+      <c r="B52" s="18">
         <f>C49+B50</f>
-        <v>0.27984457343406577</v>
+        <v>0.81895084409384578</v>
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="22" t="s">
+      <c r="A54" s="21" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1379,8 +1387,8 @@
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="24"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="23"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="10" t="s">
@@ -1398,26 +1406,25 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="4">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="B57" s="4">
-        <f>1-A57</f>
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="C57" s="4">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="D57" s="9">
-        <v>1.96</v>
+        <v>2.5750000000000002</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B58" s="25">
+      <c r="B58" s="24">
         <f>A57*B57*(D57/C57)^2</f>
-        <v>384.15999999999991</v>
+        <v>2652.2500000000005</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>

</xml_diff>